<commit_message>
FIX: better deal with empty cells in Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/worksheets.xlsx
+++ b/src/test/resources/worksheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="1660" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="5080" yWindow="1660" windowWidth="25040" windowHeight="17820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="3" r:id="rId1"/>
@@ -415,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -511,9 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>